<commit_message>
First Commit + Previous Test Data from end of Stage 4
</commit_message>
<xml_diff>
--- a/RPI/Test-Data/voltageSignalGenProcess.xlsx
+++ b/RPI/Test-Data/voltageSignalGenProcess.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seb\Documents\GitHub\DataLogger\Test-Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Seb\Documents\GitHub\DataLogger\RPI\Test-Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -43,6 +43,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -520,9 +523,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1398,7 +1402,562 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>voltageSignalGen!$C$2:$C$89</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="88"/>
+                <c:pt idx="0">
+                  <c:v>3354.35236671041</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>177.005401776177</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>166.63008514664099</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-134.12909329508301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-112.003418073061</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3691.8626667073499</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>151.00460829492999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-174.25531785027599</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-114.00347911007999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3337.2268440809298</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>133.00405896175999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3301.2257454145902</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>619.14389477217901</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3296.2255928220402</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-127.25388348033</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-16.8755149998474</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3185.5972167119298</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>-210.506424146244</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1585.92339854121</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3335.4767906735401</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1971.0601519821701</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3636.6109805596998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>-126.378856776635</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3820.74159978026</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>-145.25443281350101</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>-117.75359355449</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>106.62825403607199</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3332.8517105624501</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>-110.878383739738</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3329.97662282174</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3816.99148533585</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3337.1018402661198</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>186.88070314645799</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>816.02490310373196</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>-111.003387554551</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>-109.503341776787</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>-189.630787072359</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>-118.003601184118</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3831.9919431134899</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3304.47584459975</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>-76.252327036347495</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1499.5457625049501</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>-114.503494369335</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3207.72289193395</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>111.87841425824701</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3341.1019623401498</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3080.7190160832502</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1268.78872035889</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3347.97717215491</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>-218.756675923947</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>-109.003326517532</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>557.64201788384605</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3793.4907681508798</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>74.877285073397005</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>166.380077517014</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3665.36185796685</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>163.379985961485</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3348.8521988585999</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3846.4923856318801</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>177.25540940580399</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>-205.881282998138</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3275.34995574816</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>-101.253089999084</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>2369.3223059785701</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3379.8531449324</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3371.2278817102501</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>84.377574999236998</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>245.00747703482099</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>-185.38065736869399</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3393.9785760063401</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3847.6174199652</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>820.150028992584</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>775.89867854853901</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>561.76714377269798</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>-0.87502670369579105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3F65-4157-B927-3B06661FA0E9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="442022328"/>
+        <c:axId val="442021672"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="442022328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="442021672"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="442021672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="442022328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1958,6 +2517,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1991,6 +3066,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D85EDD0-3AE5-4BC6-92B9-9155303D0641}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2298,17 +3409,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -2328,7 +3439,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>43166.500324074077</v>
       </c>
       <c r="B2">
@@ -2351,7 +3462,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>43166.500335648147</v>
       </c>
       <c r="B3">
@@ -2374,7 +3485,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>43166.500358796293</v>
       </c>
       <c r="B4">
@@ -2397,7 +3508,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>43166.500381944446</v>
       </c>
       <c r="B5">
@@ -2420,7 +3531,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>43166.500393518516</v>
       </c>
       <c r="B6">
@@ -2443,7 +3554,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>43166.500416666669</v>
       </c>
       <c r="B7">
@@ -2466,7 +3577,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>43166.500439814816</v>
       </c>
       <c r="B8">
@@ -2489,7 +3600,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>43166.500451388885</v>
       </c>
       <c r="B9">
@@ -2512,7 +3623,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>43166.500474537039</v>
       </c>
       <c r="B10">
@@ -2535,7 +3646,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>43166.500497685185</v>
       </c>
       <c r="B11">
@@ -2558,7 +3669,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>43166.500509259262</v>
       </c>
       <c r="B12">
@@ -2581,7 +3692,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>43166.500532407408</v>
       </c>
       <c r="B13">
@@ -2604,7 +3715,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>43166.500555555554</v>
       </c>
       <c r="B14">
@@ -2627,7 +3738,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>43166.500567129631</v>
       </c>
       <c r="B15">
@@ -2650,7 +3761,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>43166.500590277778</v>
       </c>
       <c r="B16">
@@ -2673,7 +3784,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>43166.500613425924</v>
       </c>
       <c r="B17">
@@ -2696,7 +3807,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>43166.500625000001</v>
       </c>
       <c r="B18">
@@ -2719,7 +3830,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>43166.500648148147</v>
       </c>
       <c r="B19">
@@ -2742,7 +3853,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>43166.500671296293</v>
       </c>
       <c r="B20">
@@ -2765,7 +3876,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>43166.50068287037</v>
       </c>
       <c r="B21">
@@ -2788,7 +3899,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>43166.500706018516</v>
       </c>
       <c r="B22">
@@ -2811,7 +3922,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>43166.50072916667</v>
       </c>
       <c r="B23">
@@ -2834,7 +3945,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>43166.500752314816</v>
       </c>
       <c r="B24">
@@ -2857,7 +3968,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>43166.500763888886</v>
       </c>
       <c r="B25">
@@ -2880,7 +3991,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>43166.500787037039</v>
       </c>
       <c r="B26">
@@ -2903,7 +4014,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>43166.500810185185</v>
       </c>
       <c r="B27">
@@ -2926,7 +4037,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>43166.500821759262</v>
       </c>
       <c r="B28">
@@ -2949,7 +4060,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>43166.500844907408</v>
       </c>
       <c r="B29">
@@ -2972,7 +4083,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>43166.500868055555</v>
       </c>
       <c r="B30">
@@ -2995,7 +4106,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>43166.500879629632</v>
       </c>
       <c r="B31">
@@ -3018,7 +4129,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="2">
         <v>43166.500902777778</v>
       </c>
       <c r="B32">
@@ -3041,7 +4152,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="2">
         <v>43166.500914351855</v>
       </c>
       <c r="B33">
@@ -3064,7 +4175,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="2">
         <v>43166.500937500001</v>
       </c>
       <c r="B34">
@@ -3087,7 +4198,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35" s="2">
         <v>43166.500960648147</v>
       </c>
       <c r="B35">
@@ -3110,7 +4221,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="2">
         <v>43166.500972222224</v>
       </c>
       <c r="B36">
@@ -3133,7 +4244,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37" s="2">
         <v>43166.50099537037</v>
       </c>
       <c r="B37">
@@ -3156,7 +4267,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38" s="2">
         <v>43166.501006944447</v>
       </c>
       <c r="B38">
@@ -3179,7 +4290,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39" s="2">
         <v>43166.501018518517</v>
       </c>
       <c r="B39">
@@ -3202,7 +4313,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="A40" s="2">
         <v>43166.50104166667</v>
       </c>
       <c r="B40">
@@ -3225,7 +4336,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="2">
         <v>43166.50105324074</v>
       </c>
       <c r="B41">
@@ -3248,7 +4359,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42" s="2">
         <v>43166.501076388886</v>
       </c>
       <c r="B42">
@@ -3271,7 +4382,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43" s="2">
         <v>43166.501087962963</v>
       </c>
       <c r="B43">
@@ -3294,7 +4405,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="A44" s="2">
         <v>43166.501099537039</v>
       </c>
       <c r="B44">
@@ -3317,7 +4428,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="A45" s="2">
         <v>43166.501122685186</v>
       </c>
       <c r="B45">
@@ -3340,7 +4451,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="A46" s="2">
         <v>43166.501134259262</v>
       </c>
       <c r="B46">
@@ -3363,7 +4474,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
+      <c r="A47" s="2">
         <v>43166.501157407409</v>
       </c>
       <c r="B47">
@@ -3386,7 +4497,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
+      <c r="A48" s="2">
         <v>43166.501168981478</v>
       </c>
       <c r="B48">
@@ -3409,7 +4520,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
+      <c r="A49" s="2">
         <v>43166.501180555555</v>
       </c>
       <c r="B49">
@@ -3432,7 +4543,7 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="A50" s="2">
         <v>43166.501203703701</v>
       </c>
       <c r="B50">
@@ -3455,7 +4566,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="1">
+      <c r="A51" s="2">
         <v>43166.501215277778</v>
       </c>
       <c r="B51">
@@ -3478,7 +4589,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="1">
+      <c r="A52" s="2">
         <v>43166.501238425924</v>
       </c>
       <c r="B52">
@@ -3501,7 +4612,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="1">
+      <c r="A53" s="2">
         <v>43166.501250000001</v>
       </c>
       <c r="B53">
@@ -3524,7 +4635,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="1">
+      <c r="A54" s="2">
         <v>43166.501273148147</v>
       </c>
       <c r="B54">
@@ -3547,7 +4658,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="A55" s="2">
         <v>43166.501284722224</v>
       </c>
       <c r="B55">
@@ -3570,7 +4681,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="1">
+      <c r="A56" s="2">
         <v>43166.501296296294</v>
       </c>
       <c r="B56">
@@ -3593,7 +4704,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="1">
+      <c r="A57" s="2">
         <v>43166.501319444447</v>
       </c>
       <c r="B57">
@@ -3616,7 +4727,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="1">
+      <c r="A58" s="2">
         <v>43166.501331018517</v>
       </c>
       <c r="B58">
@@ -3639,7 +4750,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="A59" s="2">
         <v>43166.501354166663</v>
       </c>
       <c r="B59">
@@ -3662,7 +4773,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="1">
+      <c r="A60" s="2">
         <v>43166.50136574074</v>
       </c>
       <c r="B60">
@@ -3685,7 +4796,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="1">
+      <c r="A61" s="2">
         <v>43166.501377314817</v>
       </c>
       <c r="B61">
@@ -3708,7 +4819,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="1">
+      <c r="A62" s="2">
         <v>43166.501400462963</v>
       </c>
       <c r="B62">
@@ -3731,7 +4842,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="1">
+      <c r="A63" s="2">
         <v>43166.501423611109</v>
       </c>
       <c r="B63">
@@ -3754,7 +4865,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+      <c r="A64" s="2">
         <v>43166.501435185186</v>
       </c>
       <c r="B64">
@@ -3777,7 +4888,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="1">
+      <c r="A65" s="2">
         <v>43166.501446759263</v>
       </c>
       <c r="B65">
@@ -3800,7 +4911,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="1">
+      <c r="A66" s="2">
         <v>43166.501469907409</v>
       </c>
       <c r="B66">
@@ -3823,7 +4934,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="1">
+      <c r="A67" s="2">
         <v>43166.501481481479</v>
       </c>
       <c r="B67">
@@ -3846,7 +4957,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+      <c r="A68" s="2">
         <v>43166.501504629632</v>
       </c>
       <c r="B68">
@@ -3869,7 +4980,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="1">
+      <c r="A69" s="2">
         <v>43166.501516203702</v>
       </c>
       <c r="B69">
@@ -3892,7 +5003,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="1">
+      <c r="A70" s="2">
         <v>43166.501527777778</v>
       </c>
       <c r="B70">
@@ -3915,7 +5026,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="1">
+      <c r="A71" s="2">
         <v>43166.501550925925</v>
       </c>
       <c r="B71">
@@ -3938,7 +5049,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="1">
+      <c r="A72" s="2">
         <v>43166.501562500001</v>
       </c>
       <c r="B72">
@@ -3961,7 +5072,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+      <c r="A73" s="2">
         <v>43166.501585648148</v>
       </c>
       <c r="B73">
@@ -3984,7 +5095,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="1">
+      <c r="A74" s="2">
         <v>43166.501597222225</v>
       </c>
       <c r="B74">
@@ -4007,7 +5118,7 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="1">
+      <c r="A75" s="2">
         <v>43166.501608796294</v>
       </c>
       <c r="B75">
@@ -4030,7 +5141,7 @@
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
+      <c r="A76" s="2">
         <v>43166.501631944448</v>
       </c>
       <c r="B76">
@@ -4053,7 +5164,7 @@
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+      <c r="A77" s="2">
         <v>43166.501643518517</v>
       </c>
       <c r="B77">
@@ -4076,7 +5187,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+      <c r="A78" s="2">
         <v>43166.501666666663</v>
       </c>
       <c r="B78">
@@ -4099,7 +5210,7 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+      <c r="A79" s="2">
         <v>43166.50167824074</v>
       </c>
       <c r="B79">
@@ -4122,7 +5233,7 @@
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+      <c r="A80" s="2">
         <v>43166.501701388886</v>
       </c>
       <c r="B80">
@@ -4145,7 +5256,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+      <c r="A81" s="2">
         <v>43166.501712962963</v>
       </c>
       <c r="B81">
@@ -4168,7 +5279,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="A82" s="2">
         <v>43166.50172453704</v>
       </c>
       <c r="B82">
@@ -4191,7 +5302,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
+      <c r="A83" s="2">
         <v>43166.501747685186</v>
       </c>
       <c r="B83">
@@ -4214,7 +5325,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
+      <c r="A84" s="2">
         <v>43166.501759259256</v>
       </c>
       <c r="B84">
@@ -4237,7 +5348,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A85" s="1">
+      <c r="A85" s="2">
         <v>43166.501782407409</v>
       </c>
       <c r="B85">
@@ -4260,7 +5371,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="1">
+      <c r="A86" s="2">
         <v>43166.501805555556</v>
       </c>
       <c r="B86">
@@ -4283,7 +5394,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+      <c r="A87" s="2">
         <v>43166.501817129632</v>
       </c>
       <c r="B87">
@@ -4306,7 +5417,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
+      <c r="A88" s="2">
         <v>43166.501840277779</v>
       </c>
       <c r="B88">
@@ -4329,7 +5440,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
+      <c r="A89" s="2">
         <v>43166.501863425925</v>
       </c>
       <c r="B89">
@@ -4352,7 +5463,7 @@
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A90" s="1">
+      <c r="A90" s="2">
         <v>43166.501886574071</v>
       </c>
       <c r="B90">
@@ -4360,7 +5471,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A91" s="1">
+      <c r="A91" s="2">
         <v>43166.501898148148</v>
       </c>
       <c r="B91">
@@ -4368,7 +5479,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+      <c r="A92" s="2">
         <v>43166.501921296294</v>
       </c>
       <c r="B92">
@@ -4376,7 +5487,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="1">
+      <c r="A93" s="2">
         <v>43166.501944444448</v>
       </c>
       <c r="B93">
@@ -4384,7 +5495,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A94" s="1">
+      <c r="A94" s="2">
         <v>43166.501956018517</v>
       </c>
       <c r="B94">
@@ -4392,7 +5503,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="1">
+      <c r="A95" s="2">
         <v>43166.501979166664</v>
       </c>
       <c r="B95">
@@ -4400,7 +5511,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
+      <c r="A96" s="2">
         <v>43166.502002314817</v>
       </c>
       <c r="B96">
@@ -4408,7 +5519,7 @@
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+      <c r="A97" s="2">
         <v>43166.502013888887</v>
       </c>
       <c r="B97">
@@ -4416,7 +5527,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1">
+      <c r="A98" s="2">
         <v>43166.50203703704</v>
       </c>
       <c r="B98">
@@ -4424,7 +5535,7 @@
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1">
+      <c r="A99" s="2">
         <v>43166.502060185187</v>
       </c>
       <c r="B99">
@@ -4432,7 +5543,7 @@
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1">
+      <c r="A100" s="2">
         <v>43166.502071759256</v>
       </c>
       <c r="B100">
@@ -4440,7 +5551,7 @@
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1">
+      <c r="A101" s="2">
         <v>43166.50209490741</v>
       </c>
       <c r="B101">
@@ -4448,7 +5559,7 @@
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+      <c r="A102" s="2">
         <v>43166.502118055556</v>
       </c>
       <c r="B102">
@@ -4456,7 +5567,7 @@
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1">
+      <c r="A103" s="2">
         <v>43166.502141203702</v>
       </c>
       <c r="B103">
@@ -4464,7 +5575,7 @@
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1">
+      <c r="A104" s="2">
         <v>43166.502152777779</v>
       </c>
       <c r="B104">
@@ -4472,7 +5583,7 @@
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1">
+      <c r="A105" s="2">
         <v>43166.502175925925</v>
       </c>
       <c r="B105">
@@ -4480,7 +5591,7 @@
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1">
+      <c r="A106" s="2">
         <v>43166.502199074072</v>
       </c>
       <c r="B106">
@@ -4488,7 +5599,7 @@
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+      <c r="A107" s="2">
         <v>43166.502210648148</v>
       </c>
       <c r="B107">
@@ -4496,7 +5607,7 @@
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1">
+      <c r="A108" s="2">
         <v>43166.502233796295</v>
       </c>
       <c r="B108">
@@ -4504,7 +5615,7 @@
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1">
+      <c r="A109" s="2">
         <v>43166.502245370371</v>
       </c>
       <c r="B109">
@@ -4512,7 +5623,7 @@
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1">
+      <c r="A110" s="2">
         <v>43166.502268518518</v>
       </c>
       <c r="B110">
@@ -4520,7 +5631,7 @@
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1">
+      <c r="A111" s="2">
         <v>43166.502280092594</v>
       </c>
       <c r="B111">
@@ -4528,7 +5639,7 @@
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1">
+      <c r="A112" s="2">
         <v>43166.502303240741</v>
       </c>
       <c r="B112">
@@ -4536,7 +5647,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="1">
+      <c r="A113" s="2">
         <v>43166.502314814818</v>
       </c>
       <c r="B113">
@@ -4544,7 +5655,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="1">
+      <c r="A114" s="2">
         <v>43166.502337962964</v>
       </c>
       <c r="B114">
@@ -11296,6 +12407,7 @@
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>